<commit_message>
Added variable RPEpUACE. Confirm this data accurately represents the variable.
</commit_message>
<xml_diff>
--- a/InputData/land/RPEpUACE/Rebound Pol Emis per Unit Avoided CO2 Emis.xlsx
+++ b/InputData/land/RPEpUACE/Rebound Pol Emis per Unit Avoided CO2 Emis.xlsx
@@ -1,27 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\land\RPEpUACE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/regisrathmann/Documents/WRI/Produtos/Produto 4/InputData/land/RPEpUACE/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A342D9C-A4CF-FE4D-B904-271D20A181CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="383" yWindow="83" windowWidth="19140" windowHeight="9263"/>
+    <workbookView xWindow="400" yWindow="460" windowWidth="19140" windowHeight="9280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="RPEpUACE" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>RPEpUACE Rebound Pollutant Emissions per Unit Avoided CO2 Emissions</t>
   </si>
@@ -29,12 +38,6 @@
     <t>Source:</t>
   </si>
   <si>
-    <t>http://www.epa.gov/climatechange/Downloads/ghgemissions/US-GHG-Inventory-2015-Main-Text.pdf</t>
-  </si>
-  <si>
-    <t>Page 6-4, Table 6-3</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -44,21 +47,12 @@
     <t>and N2O released, mostly from forest fires, but also some from soils.</t>
   </si>
   <si>
-    <t>We use the historical relationship between net CO2 sequestration and CH4/N2O</t>
-  </si>
-  <si>
     <t>emissions to establish a relationship that we apply to future years (in the BAU case)</t>
   </si>
   <si>
     <t>and to the effects of policy levers in the model.</t>
   </si>
   <si>
-    <t>U.S. EPA</t>
-  </si>
-  <si>
-    <t>Excerpt from Table 6-3:</t>
-  </si>
-  <si>
     <t>CO2</t>
   </si>
   <si>
@@ -104,16 +98,55 @@
     <t>F gases</t>
   </si>
   <si>
-    <t>Inventory of U.S. Greenhouse Gas Emissions and Sinks: 1990-2013</t>
-  </si>
-  <si>
     <t>Rebound Emis Factor (dimensionless)</t>
+  </si>
+  <si>
+    <t>Page 184, Table 3.114</t>
+  </si>
+  <si>
+    <t>http://www.ccst.inpe.br/publicacao/terceira-comunicacao-nacional-do-brasil-a-convencao-quadro-das-nacoes-unidas-sobre-mudanca-do-clima-portugues/</t>
+  </si>
+  <si>
+    <t>3ª Comunicação Nacional do Brasil à Convenção-Quadro das Nações Unidas sobre Mudança do Clima - Volume III</t>
+  </si>
+  <si>
+    <t>Brazilian Ministry of Science, Technology, Innovation and Communication (MCTIC)</t>
+  </si>
+  <si>
+    <t>We use the historical relationship between net CO2 emission and CH4/N2O</t>
+  </si>
+  <si>
+    <t>Excerpt from Table 3.114:</t>
+  </si>
+  <si>
+    <t>The calculation on "RPEpUACE" table has been changed the signal (-) to (+).</t>
+  </si>
+  <si>
+    <t>This because CH4 and N2O emission are also positive, as CO2.</t>
+  </si>
+  <si>
+    <t>this variable should not contain "Avoided" in the name, but just CO2 emission.</t>
+  </si>
+  <si>
+    <t>For Brazil, as there is a positive amount of CO2 emitted from LULUCF (no sequestration),</t>
+  </si>
+  <si>
+    <t>CO2 emission</t>
+  </si>
+  <si>
+    <t>CH4 and N2O emission</t>
+  </si>
+  <si>
+    <t>Page 181, Table 3.111</t>
+  </si>
+  <si>
+    <t>In the same document above</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -139,12 +172,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -160,7 +199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -168,9 +207,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -187,7 +227,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -262,6 +302,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -297,6 +354,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -472,79 +546,139 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B4" s="4">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B5" t="s">
+      <c r="B3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="4">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B6" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>9</v>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -552,152 +686,152 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.19921875" customWidth="1"/>
-    <col min="2" max="2" width="8.86328125" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>1990</v>
+      </c>
+      <c r="C3">
+        <v>1995</v>
+      </c>
+      <c r="D3">
+        <v>2000</v>
+      </c>
+      <c r="E3">
+        <v>2005</v>
+      </c>
+      <c r="F3">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>756970</v>
+      </c>
+      <c r="C4">
+        <v>1837508</v>
+      </c>
+      <c r="D4">
+        <v>1197175</v>
+      </c>
+      <c r="E4">
+        <v>1797842</v>
+      </c>
+      <c r="F4">
+        <v>310736</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>1041.5</v>
+      </c>
+      <c r="C5">
+        <v>2895.7</v>
+      </c>
+      <c r="D5">
+        <v>2048.8000000000002</v>
+      </c>
+      <c r="E5">
+        <v>3237.9</v>
+      </c>
+      <c r="F5">
+        <v>1135.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>42.56</v>
+      </c>
+      <c r="C6">
+        <v>106.58</v>
+      </c>
+      <c r="D6">
+        <v>81.96</v>
+      </c>
+      <c r="E6">
+        <v>125.25</v>
+      </c>
+      <c r="F6">
+        <v>47.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B3">
-        <v>2009</v>
-      </c>
-      <c r="C3">
-        <v>2010</v>
-      </c>
-      <c r="D3">
-        <v>2011</v>
-      </c>
-      <c r="E3">
-        <v>2012</v>
-      </c>
-      <c r="F3">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>-862631</v>
-      </c>
-      <c r="C4">
-        <v>-862025</v>
-      </c>
-      <c r="D4">
-        <v>-872103</v>
-      </c>
-      <c r="E4">
-        <v>-869580</v>
-      </c>
-      <c r="F4">
-        <v>-871026</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>234</v>
-      </c>
-      <c r="C5">
-        <v>190</v>
-      </c>
-      <c r="D5">
-        <v>584</v>
-      </c>
-      <c r="E5">
-        <v>627</v>
-      </c>
-      <c r="F5">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6">
-        <v>22</v>
-      </c>
-      <c r="C6">
-        <v>20</v>
-      </c>
-      <c r="D6">
-        <v>42</v>
-      </c>
-      <c r="E6">
-        <v>45</v>
-      </c>
-      <c r="F6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>16</v>
       </c>
       <c r="B8" s="3">
         <f>B5/B4</f>
-        <v>-2.7126314727850032E-4</v>
+        <v>1.3758801537709553E-3</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ref="C8:F8" si="0">C5/C4</f>
-        <v>-2.2041124097328964E-4</v>
+        <v>1.575884295469734E-3</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="0"/>
-        <v>-6.6964567258683894E-4</v>
+        <v>1.7113621650969993E-3</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" si="0"/>
-        <v>-7.2103774235837996E-4</v>
+        <v>1.8009925232584398E-3</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
-        <v>-2.6750062569888842E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+        <v>3.6542273827300346E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B9" s="3">
         <f>B6/B4</f>
-        <v>-2.5503372821055586E-5</v>
+        <v>5.6224156835805914E-5</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ref="C9:F9" si="1">C6/C4</f>
-        <v>-2.3201183260346277E-5</v>
+        <v>5.8002468560681098E-5</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" si="1"/>
-        <v>-4.8159449055902798E-5</v>
+        <v>6.8461169002025598E-5</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="1"/>
-        <v>-5.1749120264955494E-5</v>
+        <v>6.9666856153099106E-5</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="1"/>
-        <v>-2.6405641163409588E-5</v>
+        <v>1.515112507079965E-4</v>
       </c>
     </row>
   </sheetData>
@@ -706,119 +840,119 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3">
+        <f>AVERAGE(Data!B8:F8)</f>
+        <v>2.0236693040652327E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3">
+        <f>AVERAGE(Data!B9:F9)</f>
+        <v>8.0773180251921632E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>21</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="3">
-        <f>-AVERAGE(Data!B8:F8)</f>
-        <v>4.2997168577917945E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="3">
-        <f>-AVERAGE(Data!B9:F9)</f>
-        <v>3.5003753313133949E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>26</v>
       </c>
       <c r="B13">
         <v>0</v>

</xml_diff>